<commit_message>
final program for term paper
</commit_message>
<xml_diff>
--- a/розрахунок вартості шаблон.xlsx
+++ b/розрахунок вартості шаблон.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учеба\7_семестр\курсавая\term_paper_3d_grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45E97EE-A5CC-4512-9E92-B1C260A0673D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6DC36D-9CB6-4A18-8B82-8B66074FB884}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Контингент студентів</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>вартість контракту</t>
+  </si>
+  <si>
+    <t>усього витрат на студента</t>
   </si>
 </sst>
 </file>
@@ -588,277 +591,277 @@
             <c:numRef>
               <c:f>'загальна вартість'!$I$3:$I$92</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>35000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -892,277 +895,277 @@
             <c:numRef>
               <c:f>'загальна вартість'!$H$3:$H$92</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1941,10 +1944,10 @@
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>106424</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>115651</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1955,7 +1958,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2293,13 +2298,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
+      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2319,7 @@
     <col min="28" max="28" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2344,7 +2349,7 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="6"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2374,7 +2379,7 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -2458,6 +2463,9 @@
       </c>
       <c r="AB3" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2468,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097DE100-1A72-44D2-B34E-8D802EAD06D6}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,7 +2494,7 @@
     <col min="28" max="28" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2516,7 +2524,7 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="6"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2546,7 +2554,7 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="2" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -2630,6 +2638,9 @@
       </c>
       <c r="AB3" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2641,8 +2652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41ECE9A-CF81-4A99-9873-07B387EA162D}">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,11 +2728,13 @@
         <f t="shared" ref="G3:G66" si="0">F3/$G$1</f>
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>70000</v>
-      </c>
-      <c r="I3">
-        <v>35000</v>
+      <c r="H3" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2752,11 +2765,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>70000</v>
-      </c>
-      <c r="I4">
-        <v>35000</v>
+      <c r="H4" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2787,11 +2802,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>70000</v>
-      </c>
-      <c r="I5">
-        <v>35000</v>
+      <c r="H5" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2822,11 +2839,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>70000</v>
-      </c>
-      <c r="I6">
-        <v>35000</v>
+      <c r="H6" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2857,11 +2876,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>70000</v>
-      </c>
-      <c r="I7">
-        <v>35000</v>
+      <c r="H7" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2892,11 +2913,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>70000</v>
-      </c>
-      <c r="I8">
-        <v>35000</v>
+      <c r="H8" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2927,11 +2950,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>70000</v>
-      </c>
-      <c r="I9">
-        <v>35000</v>
+      <c r="H9" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2962,11 +2987,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>70000</v>
-      </c>
-      <c r="I10">
-        <v>35000</v>
+      <c r="H10" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2997,11 +3024,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>70000</v>
-      </c>
-      <c r="I11">
-        <v>35000</v>
+      <c r="H11" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3032,11 +3061,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12">
-        <v>70000</v>
-      </c>
-      <c r="I12">
-        <v>35000</v>
+      <c r="H12" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3067,11 +3098,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>70000</v>
-      </c>
-      <c r="I13">
-        <v>35000</v>
+      <c r="H13" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3102,11 +3135,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14">
-        <v>70000</v>
-      </c>
-      <c r="I14">
-        <v>35000</v>
+      <c r="H14" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3137,11 +3172,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15">
-        <v>70000</v>
-      </c>
-      <c r="I15">
-        <v>35000</v>
+      <c r="H15" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3172,11 +3209,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16">
-        <v>70000</v>
-      </c>
-      <c r="I16">
-        <v>35000</v>
+      <c r="H16" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3207,11 +3246,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17">
-        <v>70000</v>
-      </c>
-      <c r="I17">
-        <v>35000</v>
+      <c r="H17" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3242,11 +3283,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18">
-        <v>70000</v>
-      </c>
-      <c r="I18">
-        <v>35000</v>
+      <c r="H18" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3277,11 +3320,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19">
-        <v>70000</v>
-      </c>
-      <c r="I19">
-        <v>35000</v>
+      <c r="H19" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3312,11 +3357,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20">
-        <v>70000</v>
-      </c>
-      <c r="I20">
-        <v>35000</v>
+      <c r="H20" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3347,11 +3394,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21">
-        <v>70000</v>
-      </c>
-      <c r="I21">
-        <v>35000</v>
+      <c r="H21" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3382,11 +3431,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22">
-        <v>70000</v>
-      </c>
-      <c r="I22">
-        <v>35000</v>
+      <c r="H22" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3417,11 +3468,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23">
-        <v>70000</v>
-      </c>
-      <c r="I23">
-        <v>35000</v>
+      <c r="H23" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3452,11 +3505,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24">
-        <v>70000</v>
-      </c>
-      <c r="I24">
-        <v>35000</v>
+      <c r="H24" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3487,11 +3542,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25">
-        <v>70000</v>
-      </c>
-      <c r="I25">
-        <v>35000</v>
+      <c r="H25" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3522,11 +3579,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26">
-        <v>70000</v>
-      </c>
-      <c r="I26">
-        <v>35000</v>
+      <c r="H26" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3557,11 +3616,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27">
-        <v>70000</v>
-      </c>
-      <c r="I27">
-        <v>35000</v>
+      <c r="H27" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3592,11 +3653,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28">
-        <v>70000</v>
-      </c>
-      <c r="I28">
-        <v>35000</v>
+      <c r="H28" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3627,11 +3690,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29">
-        <v>70000</v>
-      </c>
-      <c r="I29">
-        <v>35000</v>
+      <c r="H29" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3662,11 +3727,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H30">
-        <v>70000</v>
-      </c>
-      <c r="I30">
-        <v>35000</v>
+      <c r="H30" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3697,11 +3764,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31">
-        <v>70000</v>
-      </c>
-      <c r="I31">
-        <v>35000</v>
+      <c r="H31" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3732,11 +3801,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32">
-        <v>70000</v>
-      </c>
-      <c r="I32">
-        <v>35000</v>
+      <c r="H32" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3767,11 +3838,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H33">
-        <v>70000</v>
-      </c>
-      <c r="I33">
-        <v>35000</v>
+      <c r="H33" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3802,11 +3875,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34">
-        <v>70000</v>
-      </c>
-      <c r="I34">
-        <v>35000</v>
+      <c r="H34" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3837,11 +3912,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H35">
-        <v>70000</v>
-      </c>
-      <c r="I35">
-        <v>35000</v>
+      <c r="H35" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3872,11 +3949,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H36">
-        <v>70000</v>
-      </c>
-      <c r="I36">
-        <v>35000</v>
+      <c r="H36" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3907,11 +3986,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H37">
-        <v>70000</v>
-      </c>
-      <c r="I37">
-        <v>35000</v>
+      <c r="H37" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3942,11 +4023,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H38">
-        <v>70000</v>
-      </c>
-      <c r="I38">
-        <v>35000</v>
+      <c r="H38" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3977,11 +4060,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H39">
-        <v>70000</v>
-      </c>
-      <c r="I39">
-        <v>35000</v>
+      <c r="H39" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4012,11 +4097,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H40">
-        <v>70000</v>
-      </c>
-      <c r="I40">
-        <v>35000</v>
+      <c r="H40" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4047,11 +4134,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H41">
-        <v>70000</v>
-      </c>
-      <c r="I41">
-        <v>35000</v>
+      <c r="H41" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4082,11 +4171,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H42">
-        <v>70000</v>
-      </c>
-      <c r="I42">
-        <v>35000</v>
+      <c r="H42" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4117,11 +4208,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H43">
-        <v>70000</v>
-      </c>
-      <c r="I43">
-        <v>35000</v>
+      <c r="H43" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4152,11 +4245,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H44">
-        <v>70000</v>
-      </c>
-      <c r="I44">
-        <v>35000</v>
+      <c r="H44" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4187,11 +4282,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H45">
-        <v>70000</v>
-      </c>
-      <c r="I45">
-        <v>35000</v>
+      <c r="H45" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4222,11 +4319,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H46">
-        <v>70000</v>
-      </c>
-      <c r="I46">
-        <v>35000</v>
+      <c r="H46" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4257,11 +4356,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H47">
-        <v>70000</v>
-      </c>
-      <c r="I47">
-        <v>35000</v>
+      <c r="H47" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4292,11 +4393,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H48">
-        <v>70000</v>
-      </c>
-      <c r="I48">
-        <v>35000</v>
+      <c r="H48" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4327,11 +4430,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H49">
-        <v>70000</v>
-      </c>
-      <c r="I49">
-        <v>35000</v>
+      <c r="H49" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4362,11 +4467,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H50">
-        <v>70000</v>
-      </c>
-      <c r="I50">
-        <v>35000</v>
+      <c r="H50" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4397,11 +4504,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H51">
-        <v>70000</v>
-      </c>
-      <c r="I51">
-        <v>35000</v>
+      <c r="H51" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4432,11 +4541,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H52">
-        <v>70000</v>
-      </c>
-      <c r="I52">
-        <v>35000</v>
+      <c r="H52" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4467,11 +4578,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H53">
-        <v>70000</v>
-      </c>
-      <c r="I53">
-        <v>35000</v>
+      <c r="H53" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4502,11 +4615,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H54">
-        <v>70000</v>
-      </c>
-      <c r="I54">
-        <v>35000</v>
+      <c r="H54" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4537,11 +4652,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H55">
-        <v>70000</v>
-      </c>
-      <c r="I55">
-        <v>35000</v>
+      <c r="H55" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4572,11 +4689,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H56">
-        <v>70000</v>
-      </c>
-      <c r="I56">
-        <v>35000</v>
+      <c r="H56" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4607,11 +4726,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H57">
-        <v>70000</v>
-      </c>
-      <c r="I57">
-        <v>35000</v>
+      <c r="H57" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,11 +4763,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H58">
-        <v>70000</v>
-      </c>
-      <c r="I58">
-        <v>35000</v>
+      <c r="H58" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -4677,11 +4800,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H59">
-        <v>70000</v>
-      </c>
-      <c r="I59">
-        <v>35000</v>
+      <c r="H59" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -4712,11 +4837,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H60">
-        <v>70000</v>
-      </c>
-      <c r="I60">
-        <v>35000</v>
+      <c r="H60" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -4747,11 +4874,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H61">
-        <v>70000</v>
-      </c>
-      <c r="I61">
-        <v>35000</v>
+      <c r="H61" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -4782,11 +4911,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H62">
-        <v>70000</v>
-      </c>
-      <c r="I62">
-        <v>35000</v>
+      <c r="H62" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -4817,11 +4948,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H63">
-        <v>70000</v>
-      </c>
-      <c r="I63">
-        <v>35000</v>
+      <c r="H63" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -4852,11 +4985,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H64">
-        <v>70000</v>
-      </c>
-      <c r="I64">
-        <v>35000</v>
+      <c r="H64" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -4887,11 +5022,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H65">
-        <v>70000</v>
-      </c>
-      <c r="I65">
-        <v>35000</v>
+      <c r="H65" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4922,11 +5059,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H66">
-        <v>70000</v>
-      </c>
-      <c r="I66">
-        <v>35000</v>
+      <c r="H66" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4957,11 +5096,13 @@
         <f t="shared" ref="G67:G92" si="3">F67/$G$1</f>
         <v>0</v>
       </c>
-      <c r="H67">
-        <v>70000</v>
-      </c>
-      <c r="I67">
-        <v>35000</v>
+      <c r="H67" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -4992,11 +5133,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H68">
-        <v>70000</v>
-      </c>
-      <c r="I68">
-        <v>35000</v>
+      <c r="H68" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -5027,11 +5170,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H69">
-        <v>70000</v>
-      </c>
-      <c r="I69">
-        <v>35000</v>
+      <c r="H69" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5062,11 +5207,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H70">
-        <v>70000</v>
-      </c>
-      <c r="I70">
-        <v>35000</v>
+      <c r="H70" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5097,11 +5244,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H71">
-        <v>70000</v>
-      </c>
-      <c r="I71">
-        <v>35000</v>
+      <c r="H71" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -5132,11 +5281,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H72">
-        <v>70000</v>
-      </c>
-      <c r="I72">
-        <v>35000</v>
+      <c r="H72" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I72" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -5167,11 +5318,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H73">
-        <v>70000</v>
-      </c>
-      <c r="I73">
-        <v>35000</v>
+      <c r="H73" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -5202,11 +5355,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H74">
-        <v>70000</v>
-      </c>
-      <c r="I74">
-        <v>35000</v>
+      <c r="H74" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -5237,11 +5392,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H75">
-        <v>70000</v>
-      </c>
-      <c r="I75">
-        <v>35000</v>
+      <c r="H75" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -5272,11 +5429,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H76">
-        <v>70000</v>
-      </c>
-      <c r="I76">
-        <v>35000</v>
+      <c r="H76" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -5307,11 +5466,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H77">
-        <v>70000</v>
-      </c>
-      <c r="I77">
-        <v>35000</v>
+      <c r="H77" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5342,11 +5503,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H78">
-        <v>70000</v>
-      </c>
-      <c r="I78">
-        <v>35000</v>
+      <c r="H78" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -5377,11 +5540,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H79">
-        <v>70000</v>
-      </c>
-      <c r="I79">
-        <v>35000</v>
+      <c r="H79" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -5412,11 +5577,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H80">
-        <v>70000</v>
-      </c>
-      <c r="I80">
-        <v>35000</v>
+      <c r="H80" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I80" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -5447,11 +5614,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H81">
-        <v>70000</v>
-      </c>
-      <c r="I81">
-        <v>35000</v>
+      <c r="H81" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I81" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -5482,11 +5651,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H82">
-        <v>70000</v>
-      </c>
-      <c r="I82">
-        <v>35000</v>
+      <c r="H82" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I82" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -5517,11 +5688,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H83">
-        <v>70000</v>
-      </c>
-      <c r="I83">
-        <v>35000</v>
+      <c r="H83" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I83" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -5552,11 +5725,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H84">
-        <v>70000</v>
-      </c>
-      <c r="I84">
-        <v>35000</v>
+      <c r="H84" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -5587,11 +5762,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H85">
-        <v>70000</v>
-      </c>
-      <c r="I85">
-        <v>35000</v>
+      <c r="H85" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -5622,11 +5799,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H86">
-        <v>70000</v>
-      </c>
-      <c r="I86">
-        <v>35000</v>
+      <c r="H86" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -5657,11 +5836,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H87">
-        <v>70000</v>
-      </c>
-      <c r="I87">
-        <v>35000</v>
+      <c r="H87" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -5692,11 +5873,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H88">
-        <v>70000</v>
-      </c>
-      <c r="I88">
-        <v>35000</v>
+      <c r="H88" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -5727,11 +5910,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H89">
-        <v>70000</v>
-      </c>
-      <c r="I89">
-        <v>35000</v>
+      <c r="H89" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -5762,11 +5947,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H90">
-        <v>70000</v>
-      </c>
-      <c r="I90">
-        <v>35000</v>
+      <c r="H90" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -5797,11 +5984,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H91">
-        <v>70000</v>
-      </c>
-      <c r="I91">
-        <v>35000</v>
+      <c r="H91" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -5832,11 +6021,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H92">
-        <v>70000</v>
-      </c>
-      <c r="I92">
-        <v>35000</v>
+      <c r="H92" s="1">
+        <f>'5-й курс (магістр)'!$AB$2</f>
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <f>'5-й курс (магістр)'!$AC$2</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>